<commit_message>
CIFMM-2352 , Fixes #16 : Revise SHS example 4 (bundled) and display in the list of examples
</commit_message>
<xml_diff>
--- a/output/SharedHealthSummary/practitioner-dh-base-1.xlsx
+++ b/output/SharedHealthSummary/practitioner-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4489" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4489" uniqueCount="443">
   <si>
     <t>Path</t>
   </si>
@@ -768,7 +768,7 @@
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="AHPRA registration number"/&gt;</t>
+    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="AHPRA Registration Number"/&gt;</t>
   </si>
   <si>
     <t>The namespace for the identifier value</t>
@@ -1250,7 +1250,7 @@
     <t>Details of registration with the Australian Health Practitioner Regulation Authority (AHPRA).</t>
   </si>
   <si>
-    <t>AHPRA registration number</t>
+    <t>AHPRA Registration Number</t>
   </si>
   <si>
     <t xml:space="preserve">inv-ahpra-qual-value-0:The AHPRA registration value shall start with 3 uppercase letters, followed by 10 digits. {value.matches('^[A-Z]{3}[0-9]{10}$')}
@@ -1291,6 +1291,9 @@
   </si>
   <si>
     <t>Practitioner.qualification.identifier.value</t>
+  </si>
+  <si>
+    <t>AHPRA registration number</t>
   </si>
   <si>
     <t>Practitioner.qualification.identifier.period</t>
@@ -14090,7 +14093,7 @@
         <v>123</v>
       </c>
       <c r="K113" t="s" s="2">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="L113" t="s" s="2">
         <v>186</v>
@@ -14175,7 +14178,7 @@
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" t="s" s="2">
@@ -14284,7 +14287,7 @@
     </row>
     <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" t="s" s="2">
@@ -14421,10 +14424,10 @@
         <v>144</v>
       </c>
       <c r="K116" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="L116" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M116" s="2"/>
       <c r="N116" s="2"/>
@@ -14504,7 +14507,7 @@
     </row>
     <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" t="s" s="2">
@@ -14613,7 +14616,7 @@
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" t="s" s="2">
@@ -14724,7 +14727,7 @@
     </row>
     <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" t="s" s="2">
@@ -14837,7 +14840,7 @@
     </row>
     <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" t="s" s="2">
@@ -14863,7 +14866,7 @@
         <v>123</v>
       </c>
       <c r="K120" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="L120" t="s" s="2">
         <v>167</v>
@@ -15170,7 +15173,7 @@
     </row>
     <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" t="s" s="2">
@@ -15279,7 +15282,7 @@
     </row>
     <row r="124" hidden="true">
       <c r="A124" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" t="s" s="2">
@@ -15390,7 +15393,7 @@
     </row>
     <row r="125" hidden="true">
       <c r="A125" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" t="s" s="2">
@@ -15416,13 +15419,13 @@
         <v>123</v>
       </c>
       <c r="K125" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="L125" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="M125" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="N125" s="2"/>
       <c r="O125" t="s" s="2">
@@ -15472,7 +15475,7 @@
         <v>40</v>
       </c>
       <c r="AE125" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AF125" t="s" s="2">
         <v>41</v>
@@ -15481,7 +15484,7 @@
         <v>52</v>
       </c>
       <c r="AH125" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="AI125" t="s" s="2">
         <v>40</v>
@@ -15501,7 +15504,7 @@
     </row>
     <row r="126" hidden="true">
       <c r="A126" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" t="s" s="2">
@@ -15527,13 +15530,13 @@
         <v>108</v>
       </c>
       <c r="K126" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="L126" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="M126" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="N126" s="2"/>
       <c r="O126" t="s" s="2">
@@ -15583,7 +15586,7 @@
         <v>40</v>
       </c>
       <c r="AE126" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AF126" t="s" s="2">
         <v>41</v>
@@ -15601,7 +15604,7 @@
         <v>40</v>
       </c>
       <c r="AK126" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AL126" t="s" s="2">
         <v>40</v>
@@ -15612,7 +15615,7 @@
     </row>
     <row r="127" hidden="true">
       <c r="A127" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" t="s" s="2">
@@ -15638,13 +15641,13 @@
         <v>123</v>
       </c>
       <c r="K127" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="L127" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M127" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N127" s="2"/>
       <c r="O127" t="s" s="2">
@@ -15652,7 +15655,7 @@
       </c>
       <c r="P127" s="2"/>
       <c r="Q127" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="R127" t="s" s="2">
         <v>40</v>
@@ -15694,7 +15697,7 @@
         <v>40</v>
       </c>
       <c r="AE127" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AF127" t="s" s="2">
         <v>41</v>
@@ -15723,7 +15726,7 @@
     </row>
     <row r="128">
       <c r="A128" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" t="s" s="2">
@@ -15749,16 +15752,16 @@
         <v>144</v>
       </c>
       <c r="K128" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="L128" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="M128" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N128" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="O128" t="s" s="2">
         <v>40</v>
@@ -15787,7 +15790,7 @@
       </c>
       <c r="X128" s="2"/>
       <c r="Y128" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="Z128" t="s" s="2">
         <v>40</v>
@@ -15805,7 +15808,7 @@
         <v>40</v>
       </c>
       <c r="AE128" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AF128" t="s" s="2">
         <v>41</v>
@@ -15820,13 +15823,13 @@
         <v>40</v>
       </c>
       <c r="AJ128" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="AK128" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="AL128" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="AM128" t="s" s="2">
         <v>40</v>

</xml_diff>